<commit_message>
Refactor popup.js and implement proper updating of button states. Improved communication between companion app and extension. Improved feedback during usage of extension.
</commit_message>
<xml_diff>
--- a/Samples/SampleData01.xlsx
+++ b/Samples/SampleData01.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex\source\repos\SilverShark\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex\source\repos\SilverShark\Samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C10415-CA21-4784-BB61-CC364C9455B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130641E3-C388-4698-8F3E-7D5C8CBA7956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="624" yWindow="264" windowWidth="11664" windowHeight="8232" xr2:uid="{EC87B596-BF27-4F8F-9533-20297B64E8A2}"/>
   </bookViews>
@@ -949,9 +949,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F007D599-289A-4F2A-97D6-E4BAC663EE95}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1151,7 +1149,7 @@
         <v>90123456</v>
       </c>
       <c r="C10">
-        <v>1010</v>
+        <v>6010</v>
       </c>
       <c r="D10" t="s">
         <v>20</v>

</xml_diff>